<commit_message>
- Updated BOM - Created AS5600 Breakout schematic and board
</commit_message>
<xml_diff>
--- a/Documents/bill-of-materials.xlsx
+++ b/Documents/bill-of-materials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanes\Documents\Projects\ECTE451\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3715E0BD-59CC-4635-906E-E8A8EB33654F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA8F3E-9A59-4D88-8362-79334D06E710}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,18 +21,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BillOfMaterials!$A$10:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Example!$A$10:$H$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BillOfMaterials!$A$1:$J$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BillOfMaterials!$A$1:$J$24</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Example!$A$1:$J$31</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BillOfMaterials!$10:$10</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Example!$10:$10</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
   <si>
     <t>[42]</t>
   </si>
@@ -291,19 +292,28 @@
     <t>-</t>
   </si>
   <si>
-    <t>Magnetic Encoder</t>
-  </si>
-  <si>
-    <t>Arduino Uno</t>
-  </si>
-  <si>
-    <t>SECTE Stores</t>
-  </si>
-  <si>
-    <t>Stepper Motor</t>
-  </si>
-  <si>
-    <t>Personal</t>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Teensy 3.6</t>
+  </si>
+  <si>
+    <t>AS5600-ASOM</t>
+  </si>
+  <si>
+    <t>AS5600-ASOMCT-ND</t>
+  </si>
+  <si>
+    <t>AEAT-6600-T16</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>630-AEAT-6600-T16</t>
+  </si>
+  <si>
+    <t>1568-1465-ND</t>
   </si>
 </sst>
 </file>
@@ -317,7 +327,7 @@
     <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="168" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -423,12 +433,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -628,7 +632,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -740,52 +744,77 @@
     <xf numFmtId="166" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="24" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="54">
     <dxf>
       <font>
         <b val="0"/>
@@ -811,6 +840,31 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -948,29 +1002,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
@@ -1028,200 +1059,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1806,6 +1643,249 @@
         <name val="Arial"/>
         <scheme val="major"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -3204,18 +3284,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A10:I22" totalsRowCount="1" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49">
-  <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part #" dataDxfId="17" totalsRowDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{899A7054-1CEF-4C08-A7F2-E46A292F6B96}" name="Supplier" dataDxfId="9" totalsRowDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="15" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Supplier Part Number" dataDxfId="14" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Picture" dataDxfId="12" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost" dataDxfId="11" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="0">
-      <calculatedColumnFormula>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A10:J24" totalsRowCount="1" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
+  <tableColumns count="10">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part #" dataDxfId="50" totalsRowDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="49" totalsRowDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{899A7054-1CEF-4C08-A7F2-E46A292F6B96}" name="Supplier" dataDxfId="48" totalsRowDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="47" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Supplier Part Number" dataDxfId="46" totalsRowDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Picture" dataDxfId="44" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost" dataDxfId="43" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{22770400-E5A2-449F-A766-333A389CAFBD}" name="Shipping" dataDxfId="42" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3223,29 +3304,29 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A6:C26" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A6:C26" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Revision" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Revision Summary" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Approval Date" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Revision" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Revision Summary" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Approval Date" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A10:J31" totalsRowCount="1" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A10:J31" totalsRowCount="1" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <tableColumns count="10">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Category" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part #" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Elem ID" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Color" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Units" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Picture" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Unit Cost" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Category" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part #" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Elem ID" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Color" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Units" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Picture" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Unit Cost" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>Table14[[#This Row],[Qty]]*Table14[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3483,10 +3564,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
@@ -3509,7 +3590,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="54" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="4"/>
@@ -3597,7 +3678,7 @@
       </c>
       <c r="C7" s="40">
         <f>Table1[[#Totals],[Qty]]</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -3614,7 +3695,7 @@
       </c>
       <c r="C8" s="42">
         <f>Table1[[#Totals],[Cost]]</f>
-        <v>24.259999999999998</v>
+        <v>122.78</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -3660,6 +3741,9 @@
         <v>1</v>
       </c>
       <c r="I10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="L10" s="2"/>
@@ -3683,92 +3767,119 @@
       <c r="H11" s="13">
         <v>11.32</v>
       </c>
-      <c r="I11" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
         <v>11.32</v>
       </c>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20"/>
-      <c r="B12" s="17" t="s">
-        <v>73</v>
+      <c r="A12" s="55"/>
+      <c r="B12" s="56" t="s">
+        <v>78</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="10">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="13">
-        <f>4.9+8.04</f>
-        <v>12.94</v>
-      </c>
-      <c r="I12" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
-        <v>12.94</v>
+        <v>71</v>
+      </c>
+      <c r="D12" s="56"/>
+      <c r="E12" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="62">
+        <v>4</v>
+      </c>
+      <c r="G12" s="57"/>
+      <c r="H12" s="58">
+        <v>4.03</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="59">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
+        <v>16.12</v>
       </c>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20"/>
       <c r="B13" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="10"/>
+      <c r="E13" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
-        <v>0</v>
+      <c r="H13" s="13">
+        <v>36.880000000000003</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
+        <v>36.880000000000003</v>
       </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20"/>
       <c r="B14" s="17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
-        <v>0</v>
+      <c r="E14" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="10">
+        <v>4</v>
+      </c>
+      <c r="G14" s="64"/>
+      <c r="H14" s="13">
+        <v>11.38</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
+        <v>45.52</v>
       </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20"/>
       <c r="B15" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
       <c r="G15" s="8"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
-        <v>0</v>
+      <c r="H15" s="13">
+        <f>4.9</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I15" s="13">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="J15" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
+        <v>12.94</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -3777,12 +3888,13 @@
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
+      <c r="E16" s="63"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
         <v>0</v>
       </c>
       <c r="L16" s="2"/>
@@ -3792,12 +3904,13 @@
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
+      <c r="E17" s="63"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
         <v>0</v>
       </c>
       <c r="L17" s="2"/>
@@ -3811,8 +3924,9 @@
       <c r="F18" s="10"/>
       <c r="G18" s="8"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
+      <c r="I18" s="13"/>
+      <c r="J18" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
         <v>0</v>
       </c>
       <c r="L18" s="2"/>
@@ -3826,8 +3940,9 @@
       <c r="F19" s="10"/>
       <c r="G19" s="8"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
+      <c r="I19" s="13"/>
+      <c r="J19" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
         <v>0</v>
       </c>
       <c r="L19" s="2"/>
@@ -3841,8 +3956,9 @@
       <c r="F20" s="10"/>
       <c r="G20" s="8"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
+      <c r="I20" s="13"/>
+      <c r="J20" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
         <v>0</v>
       </c>
       <c r="L20" s="2"/>
@@ -3856,38 +3972,64 @@
       <c r="F21" s="10"/>
       <c r="G21" s="8"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
+      <c r="I21" s="13"/>
+      <c r="J21" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
         <v>0</v>
       </c>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.35">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43" t="s">
+      <c r="A22" s="20"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.35">
+      <c r="A23" s="20"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="15">
+        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.35">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12">
         <f>SUBTOTAL(109,Table1[Qty])</f>
-        <v>2</v>
-      </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="46">
+        <v>11</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="16">
         <f>SUBTOTAL(109,Table1[Cost])</f>
-        <v>24.259999999999998</v>
-      </c>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E23" s="2"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E24" s="2"/>
+        <v>122.78</v>
+      </c>
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -3929,6 +4071,12 @@
     <row r="34" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E34" s="2"/>
       <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.35">
+      <c r="E36" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4980,174 +5128,174 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.59765625" style="55" customWidth="1"/>
-    <col min="2" max="2" width="66.5" style="55" customWidth="1"/>
+    <col min="1" max="1" width="2.59765625" style="51" customWidth="1"/>
+    <col min="2" max="2" width="66.5" style="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47"/>
-      <c r="B1" s="56" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="48"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="48"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="44"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="48"/>
+      <c r="C3" s="44"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="57" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="44"/>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="48"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="44"/>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="47"/>
-      <c r="B6" s="51" t="s">
+      <c r="A6" s="43"/>
+      <c r="B6" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="48"/>
+      <c r="C6" s="44"/>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="48"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="44"/>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="50" t="s">
+      <c r="A8" s="43"/>
+      <c r="B8" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="48"/>
+      <c r="C8" s="44"/>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="48"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="44"/>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="50" t="s">
+      <c r="A10" s="43"/>
+      <c r="B10" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="48"/>
+      <c r="C10" s="44"/>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="48"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="44"/>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="50" t="s">
+      <c r="A12" s="43"/>
+      <c r="B12" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="48"/>
+      <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="48"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="44"/>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="52" t="s">
+      <c r="A14" s="43"/>
+      <c r="B14" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="48"/>
+      <c r="C14" s="44"/>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="50" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="48"/>
+      <c r="C15" s="44"/>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="48"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="54" t="s">
+      <c r="A17" s="43"/>
+      <c r="B17" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="48"/>
+      <c r="C17" s="44"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="48"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="48"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="48"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="48"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="48"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="48"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="48"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="48"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Completed breakout boards and BOM
</commit_message>
<xml_diff>
--- a/Documents/bill-of-materials.xlsx
+++ b/Documents/bill-of-materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanes\Documents\Projects\ECTE451\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA8F3E-9A59-4D88-8362-79334D06E710}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781F014E-9D99-4364-B07A-5D35D34AC120}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,19 +21,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BillOfMaterials!$A$10:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Example!$A$10:$H$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BillOfMaterials!$A$1:$J$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BillOfMaterials!$A$1:$J$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Example!$A$1:$J$31</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BillOfMaterials!$10:$10</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Example!$10:$10</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="94">
   <si>
     <t>[42]</t>
   </si>
@@ -54,9 +53,6 @@
   </si>
   <si>
     <t>PLATE 1X1 ROUND</t>
-  </si>
-  <si>
-    <t>[ Product Name ]</t>
   </si>
   <si>
     <t>194 - Medium Stone Grey</t>
@@ -314,6 +310,39 @@
   </si>
   <si>
     <t>1568-1465-ND</t>
+  </si>
+  <si>
+    <t>10uF Capacitor</t>
+  </si>
+  <si>
+    <t>100nF Capacitor</t>
+  </si>
+  <si>
+    <t>1276-1007-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1096-1-ND</t>
+  </si>
+  <si>
+    <t>LED_0603</t>
+  </si>
+  <si>
+    <t>475-3118-1-ND</t>
+  </si>
+  <si>
+    <t>732-5342-ND</t>
+  </si>
+  <si>
+    <t>Pin Header</t>
+  </si>
+  <si>
+    <t>47k Resistor 0805</t>
+  </si>
+  <si>
+    <t>311-47.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>ECTE451 Kane Stoboi</t>
   </si>
 </sst>
 </file>
@@ -632,7 +661,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -796,9 +825,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -806,6 +832,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1059,6 +1098,249 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1645,249 +1927,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="55"/>
@@ -2067,50 +2106,6 @@
         <a:xfrm>
           <a:off x="8001000" y="0"/>
           <a:ext cx="1428750" cy="321469"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>742623</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>190293</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4286250" y="152400"/>
-          <a:ext cx="2619048" cy="1657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3284,18 +3279,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A10:J24" totalsRowCount="1" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A10:J22" totalsRowCount="1" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
   <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part #" dataDxfId="50" totalsRowDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="49" totalsRowDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{899A7054-1CEF-4C08-A7F2-E46A292F6B96}" name="Supplier" dataDxfId="48" totalsRowDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="47" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Supplier Part Number" dataDxfId="46" totalsRowDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Picture" dataDxfId="44" totalsRowDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost" dataDxfId="43" totalsRowDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{22770400-E5A2-449F-A766-333A389CAFBD}" name="Shipping" dataDxfId="42" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="0">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part #" dataDxfId="19" totalsRowDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{899A7054-1CEF-4C08-A7F2-E46A292F6B96}" name="Supplier" dataDxfId="17" totalsRowDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Description" dataDxfId="16" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Supplier Part Number" dataDxfId="15" totalsRowDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Picture" dataDxfId="13" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost" dataDxfId="12" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{22770400-E5A2-449F-A766-333A389CAFBD}" name="Shipping" dataDxfId="11" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3304,29 +3299,29 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A6:C26" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A6:C26" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Revision" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Revision Summary" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Approval Date" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Revision" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Revision Summary" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Approval Date" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A10:J31" totalsRowCount="1" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A10:J31" totalsRowCount="1" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40">
   <tableColumns count="10">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Category" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part #" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Elem ID" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Color" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Units" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Picture" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Unit Cost" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Category" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part #" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Elem ID" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Color" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Units" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Picture" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Unit Cost" dataDxfId="23" totalsRowDxfId="22" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>Table14[[#This Row],[Qty]]*Table14[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3564,10 +3559,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
@@ -3591,7 +3586,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1"/>
@@ -3611,14 +3606,12 @@
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
       <c r="L2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
-      <c r="B3" s="35" t="s">
-        <v>21</v>
-      </c>
+      <c r="B3" s="35"/>
       <c r="C3" s="36"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -3628,14 +3621,12 @@
       <c r="H3" s="6"/>
       <c r="I3" s="2"/>
       <c r="L3" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="37" t="s">
-        <v>20</v>
-      </c>
+      <c r="B4" s="37"/>
       <c r="C4" s="38"/>
       <c r="D4" s="14"/>
       <c r="F4" s="2"/>
@@ -3646,9 +3637,7 @@
     </row>
     <row r="5" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
-      <c r="B5" s="37" t="s">
-        <v>25</v>
-      </c>
+      <c r="B5" s="37"/>
       <c r="C5" s="38"/>
       <c r="D5" s="14"/>
       <c r="F5" s="2"/>
@@ -3659,9 +3648,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="B6" s="37" t="s">
-        <v>24</v>
-      </c>
+      <c r="B6" s="37"/>
       <c r="C6" s="39"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -3674,11 +3661,11 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="40">
         <f>Table1[[#Totals],[Qty]]</f>
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -3691,11 +3678,11 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="42">
         <f>Table1[[#Totals],[Cost]]</f>
-        <v>122.78</v>
+        <v>239.79999999999998</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -3723,16 +3710,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>4</v>
@@ -3741,27 +3728,27 @@
         <v>1</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20"/>
       <c r="B11" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="13">
@@ -3772,207 +3759,257 @@
       </c>
       <c r="J11" s="15">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>11.32</v>
+        <v>33.96</v>
       </c>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="55"/>
       <c r="B12" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G12" s="57"/>
       <c r="H12" s="58">
-        <v>4.03</v>
+        <v>5.66</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>16.12</v>
+        <v>28.3</v>
       </c>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20"/>
       <c r="B13" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="13">
-        <v>36.880000000000003</v>
+        <v>51.78</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="15">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>36.880000000000003</v>
+        <v>103.56</v>
       </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20"/>
       <c r="B14" s="17" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D14" s="17"/>
-      <c r="E14" s="60" t="s">
-        <v>82</v>
+      <c r="E14" s="28" t="s">
+        <v>85</v>
       </c>
       <c r="F14" s="10">
-        <v>4</v>
-      </c>
-      <c r="G14" s="64"/>
+        <v>20</v>
+      </c>
+      <c r="G14" s="63"/>
       <c r="H14" s="13">
-        <v>11.38</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="15">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>45.52</v>
+        <v>1.28</v>
       </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20"/>
-      <c r="B15" s="17" t="s">
-        <v>73</v>
+      <c r="A15" s="66"/>
+      <c r="B15" s="56" t="s">
+        <v>83</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="10">
-        <v>1</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="13">
-        <f>4.9</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="I15" s="13">
-        <v>8.0399999999999991</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D15" s="56"/>
+      <c r="E15" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="68">
+        <v>20</v>
+      </c>
+      <c r="G15" s="69"/>
+      <c r="H15" s="70">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="I15" s="65"/>
       <c r="J15" s="15">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>12.94</v>
+        <v>3.3200000000000003</v>
       </c>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
+      <c r="B16" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="65"/>
+      <c r="E16" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="64">
+        <v>10</v>
+      </c>
       <c r="G16" s="11"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
+      <c r="H16" s="65">
+        <v>0.437</v>
+      </c>
+      <c r="I16" s="65"/>
       <c r="J16" s="15">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>0</v>
+        <v>4.37</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="65"/>
+      <c r="E17" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="64">
+        <v>10</v>
+      </c>
       <c r="G17" s="11"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
+      <c r="H17" s="65">
+        <v>1.0469999999999999</v>
+      </c>
+      <c r="I17" s="65"/>
       <c r="J17" s="15">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>0</v>
+        <v>10.469999999999999</v>
       </c>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+      <c r="B18" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="10">
+        <v>100</v>
+      </c>
       <c r="G18" s="8"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="13">
+        <v>2.5600000000000001E-2</v>
+      </c>
       <c r="I18" s="13"/>
       <c r="J18" s="15">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>0</v>
+        <v>2.56</v>
       </c>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>80</v>
+      </c>
       <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="13"/>
+      <c r="E19" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="10">
+        <v>3</v>
+      </c>
+      <c r="G19" s="63"/>
+      <c r="H19" s="13">
+        <v>11.38</v>
+      </c>
       <c r="I19" s="13"/>
-      <c r="J19" s="15">
+      <c r="J19" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>0</v>
+        <v>34.14</v>
       </c>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>73</v>
+      </c>
       <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="10"/>
+      <c r="E20" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="10">
+        <v>2</v>
+      </c>
       <c r="G20" s="8"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="15">
+      <c r="H20" s="13">
+        <f>4.9</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I20" s="13">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="J20" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>0</v>
+        <v>17.84</v>
       </c>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20"/>
-      <c r="B21" s="17"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="65"/>
       <c r="J21" s="15">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
         <v>0</v>
@@ -3980,56 +4017,32 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.35">
-      <c r="A22" s="20"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>0</v>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12">
+        <f>SUBTOTAL(109,Table1[Qty])</f>
+        <v>175</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="16">
+        <f>SUBTOTAL(109,Table1[Cost])</f>
+        <v>239.79999999999998</v>
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.35">
-      <c r="A23" s="20"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="15">
-        <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]+Table1[[#This Row],[Shipping]]</f>
-        <v>0</v>
-      </c>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.35">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12">
-        <f>SUBTOTAL(109,Table1[Qty])</f>
-        <v>11</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="16">
-        <f>SUBTOTAL(109,Table1[Cost])</f>
-        <v>122.78</v>
-      </c>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E24" s="2"/>
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -4071,12 +4084,6 @@
     <row r="34" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E34" s="2"/>
       <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E36" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4086,7 +4093,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
-  <pageSetup fitToHeight="0" orientation="portrait" r:id="rId3"/>
+  <pageSetup scale="80" fitToHeight="0" orientation="portrait" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId4"/>
   <tableParts count="1">
@@ -4110,30 +4117,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="24"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4278,7 +4285,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4297,16 +4304,16 @@
       <c r="H2" s="5"/>
       <c r="K2" s="2"/>
       <c r="L2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="D3" s="35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -4315,16 +4322,16 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A4" s="14"/>
       <c r="D4" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -4333,7 +4340,7 @@
     <row r="5" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="14"/>
       <c r="D5" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="38"/>
       <c r="G5" s="2"/>
@@ -4343,7 +4350,7 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="D6" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="39"/>
       <c r="F6" s="1"/>
@@ -4356,7 +4363,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="D7" s="37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="40">
         <f>Table14[[#Totals],[Qty]]</f>
@@ -4372,7 +4379,7 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="D8" s="41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="42">
         <f>Table14[[#Totals],[Cost]]</f>
@@ -4396,25 +4403,25 @@
     </row>
     <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>4</v>
@@ -4423,13 +4430,13 @@
         <v>1</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="20">
         <v>50746</v>
@@ -4438,16 +4445,16 @@
         <v>4504369</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="10">
         <v>1</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="13">
@@ -4461,7 +4468,7 @@
     </row>
     <row r="12" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="20">
         <v>3024</v>
@@ -4470,16 +4477,16 @@
         <v>302401</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="13">
@@ -4493,7 +4500,7 @@
     </row>
     <row r="13" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="20">
         <v>3023</v>
@@ -4502,16 +4509,16 @@
         <v>302301</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="10">
         <v>2</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="13">
@@ -4525,7 +4532,7 @@
     </row>
     <row r="14" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="20">
         <v>3023</v>
@@ -4534,16 +4541,16 @@
         <v>4211398</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="13">
@@ -4557,7 +4564,7 @@
     </row>
     <row r="15" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="20">
         <v>3794</v>
@@ -4569,13 +4576,13 @@
         <v>5</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="13">
@@ -4589,7 +4596,7 @@
     </row>
     <row r="16" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="20">
         <v>3623</v>
@@ -4598,16 +4605,16 @@
         <v>362301</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="13">
@@ -4621,7 +4628,7 @@
     </row>
     <row r="17" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="20">
         <v>3623</v>
@@ -4630,16 +4637,16 @@
         <v>362321</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="13">
@@ -4653,7 +4660,7 @@
     </row>
     <row r="18" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="20">
         <v>94148</v>
@@ -4662,16 +4669,16 @@
         <v>302201</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="13">
@@ -4685,7 +4692,7 @@
     </row>
     <row r="19" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="20">
         <v>6141</v>
@@ -4697,13 +4704,13 @@
         <v>6</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="13">
@@ -4717,7 +4724,7 @@
     </row>
     <row r="20" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="20">
         <v>3070</v>
@@ -4726,16 +4733,16 @@
         <v>307021</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F20" s="10">
         <v>4</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="13">
@@ -4749,7 +4756,7 @@
     </row>
     <row r="21" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="20">
         <v>2412</v>
@@ -4758,16 +4765,16 @@
         <v>241201</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="10">
         <v>1</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="13">
@@ -4781,7 +4788,7 @@
     </row>
     <row r="22" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="20">
         <v>6019</v>
@@ -4790,16 +4797,16 @@
         <v>4538353</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="10">
         <v>4</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="13">
@@ -4813,7 +4820,7 @@
     </row>
     <row r="23" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="20">
         <v>2431</v>
@@ -4822,16 +4829,16 @@
         <v>4558168</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" s="10">
         <v>1</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="13">
@@ -4845,7 +4852,7 @@
     </row>
     <row r="24" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="20">
         <v>63868</v>
@@ -4854,16 +4861,16 @@
         <v>4535737</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="10">
         <v>4</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="13">
@@ -4877,7 +4884,7 @@
     </row>
     <row r="25" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="20">
         <v>2540</v>
@@ -4886,16 +4893,16 @@
         <v>4211632</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" s="10">
         <v>4</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="13">
@@ -4909,7 +4916,7 @@
     </row>
     <row r="26" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="20">
         <v>3176</v>
@@ -4918,16 +4925,16 @@
         <v>4225733</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="13">
@@ -4941,7 +4948,7 @@
     </row>
     <row r="27" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="20">
         <v>49668</v>
@@ -4950,16 +4957,16 @@
         <v>4224793</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="13">
@@ -4973,7 +4980,7 @@
     </row>
     <row r="28" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="20">
         <v>32123</v>
@@ -4982,16 +4989,16 @@
         <v>4211573</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" s="10">
         <v>4</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="13">
@@ -5005,7 +5012,7 @@
     </row>
     <row r="29" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="20">
         <v>6590</v>
@@ -5014,16 +5021,16 @@
         <v>4211622</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" s="10">
         <v>8</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="13">
@@ -5037,7 +5044,7 @@
     </row>
     <row r="30" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="20">
         <v>3957</v>
@@ -5046,16 +5053,16 @@
         <v>4211473</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" s="10">
         <v>4</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="13">
@@ -5072,7 +5079,7 @@
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="12">
@@ -5135,7 +5142,7 @@
     <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="43"/>
       <c r="B1" s="52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="44"/>
     </row>
@@ -5147,14 +5154,14 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="43"/>
       <c r="B3" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="44"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" s="53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="44"/>
     </row>
@@ -5166,7 +5173,7 @@
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="43"/>
       <c r="B6" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="44"/>
     </row>
@@ -5178,7 +5185,7 @@
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="43"/>
       <c r="B8" s="46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="44"/>
     </row>
@@ -5190,7 +5197,7 @@
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="44"/>
     </row>
@@ -5202,7 +5209,7 @@
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="44"/>
     </row>
@@ -5214,14 +5221,14 @@
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="44"/>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="43"/>
       <c r="B15" s="46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="44"/>
     </row>
@@ -5233,7 +5240,7 @@
     <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A17" s="43"/>
       <c r="B17" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="44"/>
     </row>

</xml_diff>